<commit_message>
New translations s.xlsx (Multilingual)
</commit_message>
<xml_diff>
--- a/fr/S.xlsx
+++ b/fr/S.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
   <si>
     <t>identifiers</t>
   </si>
@@ -50,6 +50,9 @@
     <t>Save as...</t>
   </si>
   <si>
+    <t>Speichern als...</t>
+  </si>
+  <si>
     <t>olianore</t>
   </si>
   <si>
@@ -59,64 +62,190 @@
     <t>View</t>
   </si>
   <si>
+    <t>Ansicht</t>
+  </si>
+  <si>
+    <t>Ver</t>
+  </si>
+  <si>
+    <t>cava</t>
+  </si>
+  <si>
     <t>About...</t>
   </si>
   <si>
+    <t>Über...</t>
+  </si>
+  <si>
+    <t>Acerca de...</t>
+  </si>
+  <si>
+    <t>À propos...</t>
+  </si>
+  <si>
     <t>About Me</t>
   </si>
   <si>
+    <t>Über mich</t>
+  </si>
+  <si>
+    <t>Acerca de mí</t>
+  </si>
+  <si>
+    <t>À propos de moi</t>
+  </si>
+  <si>
     <t>Current Password</t>
   </si>
   <si>
+    <t>Aktuelles Passwort</t>
+  </si>
+  <si>
+    <t>Contraseña actual</t>
+  </si>
+  <si>
+    <t>Mot de passe actuel</t>
+  </si>
+  <si>
     <t>New Password</t>
   </si>
   <si>
+    <t>Neues Passwort</t>
+  </si>
+  <si>
+    <t>Nueva contraseña</t>
+  </si>
+  <si>
     <t>Confirm New Password</t>
   </si>
   <si>
+    <t>Neues Passwort bestätigen</t>
+  </si>
+  <si>
+    <t>Confirmar nueva contraseña</t>
+  </si>
+  <si>
     <t>Change Password</t>
   </si>
   <si>
+    <t>Passwort ändern</t>
+  </si>
+  <si>
+    <t>Cambiar contraseña</t>
+  </si>
+  <si>
     <t>Password recover</t>
   </si>
   <si>
+    <t>Readeooooo messageiooooo</t>
+  </si>
+  <si>
     <t>Your password reseted successully!</t>
   </si>
   <si>
     <t>Read message</t>
   </si>
   <si>
+    <t>Nachricht lesen</t>
+  </si>
+  <si>
+    <t>Leer mensaje</t>
+  </si>
+  <si>
     <t>Are you sure you want to delete this message?</t>
   </si>
   <si>
+    <t>Sind Sie sicher, dass Sie diese Nachricht löschen möchten?</t>
+  </si>
+  <si>
+    <t>¿Está seguro que desea eliminar este mensaje?</t>
+  </si>
+  <si>
     <t>Search in messages</t>
   </si>
   <si>
+    <t>In Nachrichten suchen</t>
+  </si>
+  <si>
+    <t>Buscar en mensajes</t>
+  </si>
+  <si>
     <t>Compose Message</t>
   </si>
   <si>
+    <t>Nachricht verfassen</t>
+  </si>
+  <si>
+    <t>Redactar mensaje</t>
+  </si>
+  <si>
     <t>No date provided</t>
   </si>
   <si>
+    <t>Kein Datum angegeben</t>
+  </si>
+  <si>
+    <t>No hay fecha proporcionadada</t>
+  </si>
+  <si>
     <t>Quick Start</t>
   </si>
   <si>
+    <t>Schnellstart</t>
+  </si>
+  <si>
+    <t>Inicio rápido</t>
+  </si>
+  <si>
     <t>Identifier</t>
   </si>
   <si>
     <t>Text for translation 1</t>
   </si>
   <si>
+    <t xml:space="preserve"> Traduction 1</t>
+  </si>
+  <si>
+    <t>Traducción 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Traducción 1</t>
+  </si>
+  <si>
     <t>Text for translation 2</t>
   </si>
   <si>
+    <t>Traduction 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Traducción 2</t>
+  </si>
+  <si>
     <t>Text for translation 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Traduction 3 </t>
+  </si>
+  <si>
+    <t>Traducción 3</t>
+  </si>
+  <si>
     <t>Text for translation 4</t>
   </si>
   <si>
+    <t>Traduction 4</t>
+  </si>
+  <si>
+    <t>Traducción 4</t>
+  </si>
+  <si>
     <t>Text for translation 5</t>
+  </si>
+  <si>
+    <t>Traduction 5</t>
+  </si>
+  <si>
+    <t>Traducción 5</t>
   </si>
 </sst>
 </file>
@@ -639,16 +768,16 @@
         <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,19 +785,19 @@
         <v>535</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -676,19 +805,19 @@
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -696,19 +825,19 @@
         <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,19 +845,19 @@
         <v>786</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,19 +865,19 @@
         <v>786</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -756,19 +885,19 @@
         <v>76</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,19 +905,19 @@
         <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,19 +925,19 @@
         <v>6464</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -816,19 +945,19 @@
         <v>646</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="F12" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -836,19 +965,19 @@
         <v>6464</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,19 +985,19 @@
         <v>786</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -876,19 +1005,19 @@
         <v>57657</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -896,19 +1025,19 @@
         <v>545</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,19 +1045,19 @@
         <v>545765</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -936,19 +1065,19 @@
         <v>5745465</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -968,7 +1097,7 @@
   <sheetData>
     <row r="1" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -991,19 +1120,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1011,19 +1140,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1031,19 +1160,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1051,19 +1180,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1071,19 +1200,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>